<commit_message>
remove data - notebooks folders
</commit_message>
<xml_diff>
--- a/data/DiccionarioDatos_18.xlsx
+++ b/data/DiccionarioDatos_18.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\PNDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amosluna/Desktop/diplomado_ia_pucp/final_projects/PDS_mod1_diplom_ai_pucp_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB653DE1-4E31-1B45-93F4-6E295829F32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView minimized="1" xWindow="34560" yWindow="3040" windowWidth="47540" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiccionarioDatos" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Variable</t>
   </si>
@@ -72,9 +73,6 @@
   </si>
   <si>
     <t>MAGNITUD</t>
-  </si>
-  <si>
-    <t>Hora universal coordinada (UTC), cinco horas adelantadas con respecto a la hora local debido a que Peru se encuentra en una zona horaria UTC -5</t>
   </si>
   <si>
     <t>Es la distancia en grados, minutos y segundos que hay con respecto al meridiano principal, que es el meridiano de Greenwich (0º).</t>
@@ -104,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,10 +186,10 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,32 +529,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="84.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1"/>
-    <col min="5" max="5" width="26.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="20.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1"/>
+    <col min="5" max="5" width="26.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -573,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -590,12 +588,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>7</v>
@@ -607,13 +605,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
@@ -621,40 +617,40 @@
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>7</v>
@@ -662,15 +658,15 @@
       <c r="D10" s="10"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="5"/>

</xml_diff>